<commit_message>
journal de travail Winston
</commit_message>
<xml_diff>
--- a/Semaine 4/Journal de travail - Winston Meisen.xlsx
+++ b/Semaine 4/Journal de travail - Winston Meisen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Tâche effectuées</t>
   </si>
@@ -82,6 +82,18 @@
   <si>
     <t xml:space="preserve">Création de la partie Raid pour être ajoutée
 dans le support </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date : 30.09.2018 </t>
+  </si>
+  <si>
+    <t>Recherche sur les Raid logiciels et matériels</t>
+  </si>
+  <si>
+    <t>Mise à jour du rapport de travail</t>
+  </si>
+  <si>
+    <t>15min</t>
   </si>
 </sst>
 </file>
@@ -174,37 +186,37 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,10 +525,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:G26"/>
+  <dimension ref="B3:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C23"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,24 +538,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -560,239 +572,274 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="9"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="F22:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="B13:C14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B22:C23"/>
+  <mergeCells count="42">
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:G31"/>
     <mergeCell ref="D15:E16"/>
     <mergeCell ref="D17:E18"/>
     <mergeCell ref="D22:E23"/>
@@ -806,6 +853,28 @@
     <mergeCell ref="D25:E26"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="D13:E14"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>